<commit_message>
added error-causing files to notes.html
</commit_message>
<xml_diff>
--- a/data/approval.xlsx
+++ b/data/approval.xlsx
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -485,10 +485,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -501,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -510,10 +510,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -535,10 +535,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -548,7 +548,7 @@
         </is>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -563,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -576,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -585,10 +585,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -613,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -626,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -635,10 +635,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="B9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -663,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -676,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -685,10 +685,10 @@
         <v>0</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -710,10 +710,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -735,10 +735,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -751,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -760,10 +760,10 @@
         <v>0</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -785,10 +785,10 @@
         <v>0</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -801,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -810,10 +810,10 @@
         <v>0</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
satisfaction stuff staat nu in 1 functie
</commit_message>
<xml_diff>
--- a/data/approval.xlsx
+++ b/data/approval.xlsx
@@ -462,22 +462,22 @@
         <v>6</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -485,13 +485,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -508,22 +508,22 @@
         <v>8</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -531,22 +531,22 @@
         <v>9</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
       <c r="G5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -554,22 +554,22 @@
         <v>10</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -577,22 +577,22 @@
         <v>11</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -600,13 +600,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -623,22 +623,22 @@
         <v>13</v>
       </c>
       <c r="B9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
       </c>
       <c r="D9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -646,13 +646,13 @@
         <v>14</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -669,13 +669,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -692,22 +692,22 @@
         <v>16</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -715,13 +715,13 @@
         <v>17</v>
       </c>
       <c r="B13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -738,13 +738,13 @@
         <v>18</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -761,13 +761,13 @@
         <v>19</v>
       </c>
       <c r="B15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>

</xml_diff>